<commit_message>
add redirection to the family page code
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27318"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aotenant1-my.sharepoint.com/personal/indrajeet_bind_agingoptions_com/Documents/Project/Automation_AOLogin/agingoptions/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AO\Desktop\AO Framework\Automation_AO\agingoptions\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:801_{C9F0A2DD-194A-4E7D-8CD6-32616010F772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{247C62BE-3F33-4474-A03E-0200DD68FD0A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="137">
   <si>
     <t>S.N.</t>
   </si>
@@ -261,12 +260,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>verify_TC002_ValidLogin</t>
-  </si>
-  <si>
-    <t>TC-002</t>
-  </si>
-  <si>
     <t>userName/Email</t>
   </si>
   <si>
@@ -421,13 +414,46 @@
   </si>
   <si>
     <t>TC-014</t>
+  </si>
+  <si>
+    <t>Family_TC002</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>Mohan</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>Verma</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mohankumar@maildrop.cc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +489,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -485,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -493,6 +527,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -512,9 +548,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -552,9 +588,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -589,7 +625,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -624,7 +660,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -797,290 +833,310 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+    <col min="2" max="2" width="59.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73">
-      <c r="A1" t="s">
+    <row r="1" spans="1:73" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AK1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AL1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AM1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AO1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AP1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AR1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AS1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AT1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AU1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AV1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AX1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AY1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="AZ1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BA1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BB1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BC1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BD1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BE1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BF1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BG1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BH1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BI1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BJ1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BK1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BL1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BM1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BN1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BO1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BP1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BQ1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BR1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BS1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BT1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BU1" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:73" ht="23.1">
+    <row r="2" spans="1:73" ht="23" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="M2" s="4"/>
-      <c r="O2" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="H2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" s="7">
+        <v>37593</v>
+      </c>
+      <c r="L2" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="4">
+        <v>8090796943</v>
+      </c>
+      <c r="N2" t="s">
+        <v>135</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:73" ht="23.1">
+    <row r="3" spans="1:73" ht="23" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="C3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="I3" s="3"/>
       <c r="K3" s="3"/>
@@ -1088,290 +1144,291 @@
       <c r="O3" s="1"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:73" ht="23.1">
+    <row r="4" spans="1:73" ht="23" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" t="s">
-        <v>78</v>
-      </c>
       <c r="G4" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M4" s="1"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:73">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="D5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:73">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="D6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:73">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>100</v>
       </c>
-      <c r="D7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="G7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" t="s">
         <v>101</v>
       </c>
-      <c r="F7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H7" t="s">
-        <v>103</v>
-      </c>
       <c r="I7" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:73">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J10" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H8" t="s">
-        <v>103</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>79</v>
+      <c r="G11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s">
+        <v>118</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:73">
-      <c r="A9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" t="s">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>110</v>
+      <c r="E12" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:73">
-      <c r="A10" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H10" t="s">
-        <v>103</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="J10" t="s">
-        <v>116</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:73">
-      <c r="A11" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="F11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" t="s">
-        <v>120</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:73">
-      <c r="A12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:73">
-      <c r="A13" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{512DE707-263F-44B4-9676-A132F7D7D495}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{A5EF5095-7E51-46DF-9992-73D0B45BAA66}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{D29CE209-7365-4D21-B50C-ECE07F6D1AFE}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{6F81BE04-C7E4-417E-9CF5-CE3F5D45A315}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{102F1BCB-D904-4D58-9341-AF78CA8C2408}"/>
-    <hyperlink ref="G4" r:id="rId6" xr:uid="{D737794A-2D56-45BA-B2EC-0121AFB1E61B}"/>
-    <hyperlink ref="E5" r:id="rId7" xr:uid="{BD8DF43A-1E7F-4CBA-8028-8E56A2E22A5C}"/>
-    <hyperlink ref="G5" r:id="rId8" xr:uid="{7937C142-A7F1-401A-AB9E-5485303ED0CA}"/>
-    <hyperlink ref="E6" r:id="rId9" xr:uid="{A34CC373-4031-4BEF-A020-F3C093C8CA87}"/>
-    <hyperlink ref="G6" r:id="rId10" xr:uid="{1CCC87D6-F3E2-4589-B668-75AF1568B023}"/>
-    <hyperlink ref="I7" r:id="rId11" xr:uid="{61C9A85D-4C57-4FE5-8B84-684E9A5C373C}"/>
-    <hyperlink ref="G7" r:id="rId12" xr:uid="{6FA6DC48-9A0D-4F82-82BE-7F4E08A45087}"/>
-    <hyperlink ref="I8" r:id="rId13" xr:uid="{841C38D4-B9C6-416F-9236-3677F7D11A20}"/>
-    <hyperlink ref="G8" r:id="rId14" xr:uid="{1178994B-1798-4AD8-A2F8-B5D03AAB3107}"/>
-    <hyperlink ref="E9" r:id="rId15" xr:uid="{1B0A9609-1A02-4495-84CD-05EFAAA57523}"/>
-    <hyperlink ref="I10" r:id="rId16" xr:uid="{4D8E4E47-DBBB-4AB1-8FE3-8851F8E7A3AF}"/>
-    <hyperlink ref="G10" r:id="rId17" xr:uid="{EB80F059-479C-4A3D-BCEA-47607E1DA109}"/>
-    <hyperlink ref="K10" r:id="rId18" xr:uid="{261AE63E-2363-422D-B0B4-53181EA13EA9}"/>
-    <hyperlink ref="G11" r:id="rId19" xr:uid="{6B6BBCB9-145F-4BE5-BBE8-30D71BCE7B48}"/>
-    <hyperlink ref="E11" r:id="rId20" xr:uid="{07EC495A-1F53-48AC-8AA0-0E666A45D3EC}"/>
-    <hyperlink ref="E12" r:id="rId21" xr:uid="{895F1735-9EC7-45B1-B6A0-ABC50C505CA1}"/>
-    <hyperlink ref="E13" r:id="rId22" xr:uid="{65FA1E07-DA76-4D17-8EE2-7A523B80D4D6}"/>
+    <hyperlink ref="G2" r:id="rId1" display="Password@123"/>
+    <hyperlink ref="E2" r:id="rId2" display="jamessmith@mailinator.com"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="G4" r:id="rId6"/>
+    <hyperlink ref="E5" r:id="rId7"/>
+    <hyperlink ref="G5" r:id="rId8"/>
+    <hyperlink ref="E6" r:id="rId9"/>
+    <hyperlink ref="G6" r:id="rId10"/>
+    <hyperlink ref="I7" r:id="rId11"/>
+    <hyperlink ref="G7" r:id="rId12"/>
+    <hyperlink ref="I8" r:id="rId13"/>
+    <hyperlink ref="G8" r:id="rId14"/>
+    <hyperlink ref="E9" r:id="rId15"/>
+    <hyperlink ref="I10" r:id="rId16"/>
+    <hyperlink ref="G10" r:id="rId17"/>
+    <hyperlink ref="K10" r:id="rId18"/>
+    <hyperlink ref="G11" r:id="rId19"/>
+    <hyperlink ref="E11" r:id="rId20"/>
+    <hyperlink ref="E12" r:id="rId21"/>
+    <hyperlink ref="E13" r:id="rId22"/>
+    <hyperlink ref="O2" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added personal info redirection page
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -416,9 +416,6 @@
     <t>TC-014</t>
   </si>
   <si>
-    <t>Family_TC002</t>
-  </si>
-  <si>
     <t>firstName</t>
   </si>
   <si>
@@ -431,22 +428,25 @@
     <t>Verma</t>
   </si>
   <si>
-    <t>Kumar</t>
-  </si>
-  <si>
-    <t>middleName</t>
-  </si>
-  <si>
-    <t>dateOfBirth</t>
-  </si>
-  <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>mohankumar@maildrop.cc</t>
+  </si>
+  <si>
+    <t>mohanverma</t>
+  </si>
+  <si>
+    <t>phoneNum</t>
+  </si>
+  <si>
+    <t>8090796943</t>
+  </si>
+  <si>
+    <t>PersonalMedicalHistoryAllElementVisibility</t>
+  </si>
+  <si>
+    <t>Health_001</t>
   </si>
 </sst>
 </file>
@@ -527,8 +527,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -847,224 +847,224 @@
     <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:73" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AK1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AM1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AP1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AR1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AS1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AT1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="8" t="s">
+      <c r="AU1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AV1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="8" t="s">
+      <c r="AW1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="8" t="s">
+      <c r="AX1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="8" t="s">
+      <c r="AY1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="8" t="s">
+      <c r="AZ1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="8" t="s">
+      <c r="BA1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="8" t="s">
+      <c r="BB1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="8" t="s">
+      <c r="BC1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="BD1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="8" t="s">
+      <c r="BE1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="8" t="s">
+      <c r="BF1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="BG1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="8" t="s">
+      <c r="BH1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="8" t="s">
+      <c r="BI1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="8" t="s">
+      <c r="BJ1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="8" t="s">
+      <c r="BK1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="8" t="s">
+      <c r="BL1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="8" t="s">
+      <c r="BM1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="8" t="s">
+      <c r="BN1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="8" t="s">
+      <c r="BO1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="8" t="s">
+      <c r="BP1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="8" t="s">
+      <c r="BQ1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="8" t="s">
+      <c r="BR1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="8" t="s">
+      <c r="BS1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="8" t="s">
+      <c r="BT1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="8" t="s">
+      <c r="BU1" s="7" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1073,46 +1073,43 @@
         <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" t="s">
         <v>126</v>
       </c>
-      <c r="C2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" t="s">
         <v>128</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" t="s">
         <v>132</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="H2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="J2" t="s">
         <v>133</v>
       </c>
-      <c r="K2" s="7">
-        <v>37593</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K2" s="8" t="s">
         <v>134</v>
       </c>
       <c r="M2" s="4">
         <v>8090796943</v>
       </c>
       <c r="N2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P2" s="2"/>
     </row>
@@ -1393,32 +1390,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="Password@123"/>
-    <hyperlink ref="E2" r:id="rId2" display="jamessmith@mailinator.com"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="G3" r:id="rId4"/>
-    <hyperlink ref="E4" r:id="rId5"/>
-    <hyperlink ref="G4" r:id="rId6"/>
-    <hyperlink ref="E5" r:id="rId7"/>
-    <hyperlink ref="G5" r:id="rId8"/>
-    <hyperlink ref="E6" r:id="rId9"/>
-    <hyperlink ref="G6" r:id="rId10"/>
-    <hyperlink ref="I7" r:id="rId11"/>
-    <hyperlink ref="G7" r:id="rId12"/>
-    <hyperlink ref="I8" r:id="rId13"/>
-    <hyperlink ref="G8" r:id="rId14"/>
-    <hyperlink ref="E9" r:id="rId15"/>
-    <hyperlink ref="I10" r:id="rId16"/>
-    <hyperlink ref="G10" r:id="rId17"/>
-    <hyperlink ref="K10" r:id="rId18"/>
-    <hyperlink ref="G11" r:id="rId19"/>
-    <hyperlink ref="E11" r:id="rId20"/>
-    <hyperlink ref="E12" r:id="rId21"/>
-    <hyperlink ref="E13" r:id="rId22"/>
-    <hyperlink ref="O2" r:id="rId23"/>
+    <hyperlink ref="E2" r:id="rId1" display="jamessmith@mailinator.com"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="G3" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="G4" r:id="rId5"/>
+    <hyperlink ref="E5" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="E6" r:id="rId8"/>
+    <hyperlink ref="G6" r:id="rId9"/>
+    <hyperlink ref="I7" r:id="rId10"/>
+    <hyperlink ref="G7" r:id="rId11"/>
+    <hyperlink ref="I8" r:id="rId12"/>
+    <hyperlink ref="G8" r:id="rId13"/>
+    <hyperlink ref="E9" r:id="rId14"/>
+    <hyperlink ref="I10" r:id="rId15"/>
+    <hyperlink ref="G10" r:id="rId16"/>
+    <hyperlink ref="K10" r:id="rId17"/>
+    <hyperlink ref="G11" r:id="rId18"/>
+    <hyperlink ref="E11" r:id="rId19"/>
+    <hyperlink ref="E12" r:id="rId20"/>
+    <hyperlink ref="E13" r:id="rId21"/>
+    <hyperlink ref="O2" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
adding personal medical history test cases
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="145">
   <si>
     <t>S.N.</t>
   </si>
@@ -419,27 +419,9 @@
     <t>firstName</t>
   </si>
   <si>
-    <t>Mohan</t>
-  </si>
-  <si>
     <t>lastName</t>
   </si>
   <si>
-    <t>Verma</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>mohankumar@maildrop.cc</t>
-  </si>
-  <si>
-    <t>mohanverma</t>
-  </si>
-  <si>
-    <t>phoneNum</t>
-  </si>
-  <si>
     <t>8090796943</t>
   </si>
   <si>
@@ -447,6 +429,48 @@
   </si>
   <si>
     <t>Health_001</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>Yadav</t>
+  </si>
+  <si>
+    <t>rohityadav</t>
+  </si>
+  <si>
+    <t>userEmail</t>
+  </si>
+  <si>
+    <t>noOfChild</t>
+  </si>
+  <si>
+    <t>primaryMemberDob</t>
+  </si>
+  <si>
+    <t>spouseFirstName</t>
+  </si>
+  <si>
+    <t>Radha</t>
+  </si>
+  <si>
+    <t>spouseDob</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>565</t>
+  </si>
+  <si>
+    <t>1980-27-10</t>
+  </si>
+  <si>
+    <t>1984-21-10</t>
   </si>
 </sst>
 </file>
@@ -519,7 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -529,6 +553,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -836,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1068,50 +1093,70 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:73" ht="23" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
         <v>126</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" t="s">
         <v>127</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J2" t="s">
-        <v>133</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>134</v>
+      <c r="L2" t="s">
+        <v>136</v>
       </c>
       <c r="M2" s="4">
-        <v>8090796943</v>
+        <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>130</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P2" s="2"/>
+        <v>137</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" t="s">
+        <v>140</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="T2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="3" spans="1:73" ht="23" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
@@ -1411,10 +1456,9 @@
     <hyperlink ref="E11" r:id="rId19"/>
     <hyperlink ref="E12" r:id="rId20"/>
     <hyperlink ref="E13" r:id="rId21"/>
-    <hyperlink ref="O2" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update the test script
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="174">
   <si>
     <t>S.N.</t>
   </si>
@@ -278,12 +278,6 @@
     <t>verify_TC003_InvalidLoginWithInvalidPassword</t>
   </si>
   <si>
-    <t>TC-003</t>
-  </si>
-  <si>
-    <t>Password@12323476</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -467,10 +461,103 @@
     <t>565</t>
   </si>
   <si>
-    <t>1980-27-10</t>
-  </si>
-  <si>
-    <t>1984-21-10</t>
+    <t>1984-10-21</t>
+  </si>
+  <si>
+    <t>1980-09-19</t>
+  </si>
+  <si>
+    <t>primaryDementia</t>
+  </si>
+  <si>
+    <t>There is not Dementia.</t>
+  </si>
+  <si>
+    <t>primaryParkinson</t>
+  </si>
+  <si>
+    <t>primaryHeartDesease</t>
+  </si>
+  <si>
+    <t>Heart issue.</t>
+  </si>
+  <si>
+    <t>primaryStroke</t>
+  </si>
+  <si>
+    <t>Stroke issue.</t>
+  </si>
+  <si>
+    <t>primaryDiabetes</t>
+  </si>
+  <si>
+    <t>there is no diabetes.</t>
+  </si>
+  <si>
+    <t>primary member blood issue.</t>
+  </si>
+  <si>
+    <t>primaryElevated</t>
+  </si>
+  <si>
+    <t>this is elevated issue.</t>
+  </si>
+  <si>
+    <t>primaryGlaucoma</t>
+  </si>
+  <si>
+    <t>spouseDementia</t>
+  </si>
+  <si>
+    <t>spouse Dementia issue.</t>
+  </si>
+  <si>
+    <t>spouseParkinson</t>
+  </si>
+  <si>
+    <t>there is no parkinsons.</t>
+  </si>
+  <si>
+    <t>spouseHeartDisease</t>
+  </si>
+  <si>
+    <t>there is not spouse heart Disease.</t>
+  </si>
+  <si>
+    <t>spouseHeart</t>
+  </si>
+  <si>
+    <t>There is no Heart Disease.</t>
+  </si>
+  <si>
+    <t>spouseBloodPressure</t>
+  </si>
+  <si>
+    <t>there is not blood pressure issue</t>
+  </si>
+  <si>
+    <t>spouseElevatedCholesterol</t>
+  </si>
+  <si>
+    <t>there is not Elevated Cholesterol.</t>
+  </si>
+  <si>
+    <t>There is not Glaucome to the spouse.</t>
+  </si>
+  <si>
+    <t>Health_005</t>
+  </si>
+  <si>
+    <t>There is not Parkinson</t>
+  </si>
+  <si>
+    <t>primaryMemberBlood</t>
+  </si>
+  <si>
+    <t>There is no Glaucome</t>
+  </si>
+  <si>
+    <t>spouseGlaucome</t>
   </si>
 </sst>
 </file>
@@ -861,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,67 +1185,67 @@
         <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" t="s">
         <v>129</v>
       </c>
-      <c r="C2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="K2" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="H2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>134</v>
-      </c>
-      <c r="J2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="L2" t="s">
-        <v>136</v>
       </c>
       <c r="M2" s="4">
         <v>1</v>
       </c>
       <c r="N2" t="s">
+        <v>135</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="P2" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q2" t="s">
         <v>137</v>
       </c>
-      <c r="O2" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>138</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="T2" t="s">
         <v>139</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="T2" t="s">
-        <v>141</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>142</v>
-      </c>
     </row>
-    <row r="3" spans="1:73" ht="23" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -1166,41 +1253,114 @@
         <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>169</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>75</v>
+        <v>143</v>
+      </c>
+      <c r="E3" t="s">
+        <v>144</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="M3" s="4"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="2"/>
+        <v>145</v>
+      </c>
+      <c r="G3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H3" t="s">
+        <v>146</v>
+      </c>
+      <c r="I3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J3" t="s">
+        <v>148</v>
+      </c>
+      <c r="K3" t="s">
+        <v>149</v>
+      </c>
+      <c r="L3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M3" t="s">
+        <v>151</v>
+      </c>
+      <c r="N3" t="s">
+        <v>171</v>
+      </c>
+      <c r="O3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P3" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>154</v>
+      </c>
+      <c r="R3" t="s">
+        <v>155</v>
+      </c>
+      <c r="S3" t="s">
+        <v>172</v>
+      </c>
+      <c r="T3" t="s">
+        <v>156</v>
+      </c>
+      <c r="U3" t="s">
+        <v>157</v>
+      </c>
+      <c r="V3" t="s">
+        <v>158</v>
+      </c>
+      <c r="W3" t="s">
+        <v>159</v>
+      </c>
+      <c r="X3" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="4" spans="1:73" ht="23" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
       </c>
       <c r="D4" t="s">
         <v>74</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
         <v>76</v>
@@ -1213,76 +1373,76 @@
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
         <v>86</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" t="s">
-        <v>88</v>
       </c>
       <c r="D5" t="s">
         <v>74</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
         <v>91</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" t="s">
-        <v>93</v>
       </c>
       <c r="D6" t="s">
         <v>74</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
         <v>76</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
         <v>96</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" t="s">
-        <v>98</v>
       </c>
       <c r="D7" t="s">
         <v>74</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>77</v>
       </c>
       <c r="H7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>77</v>
@@ -1291,28 +1451,28 @@
     </row>
     <row r="8" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" t="s">
         <v>102</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" t="s">
-        <v>104</v>
       </c>
       <c r="D8" t="s">
         <v>74</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>77</v>
       </c>
       <c r="H8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>77</v>
@@ -1320,51 +1480,51 @@
     </row>
     <row r="9" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
         <v>105</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" t="s">
-        <v>107</v>
       </c>
       <c r="D9" t="s">
         <v>74</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
         <v>109</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" t="s">
-        <v>111</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" t="s">
         <v>112</v>
-      </c>
-      <c r="F10" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H10" t="s">
-        <v>101</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="J10" t="s">
-        <v>114</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>77</v>
@@ -1372,13 +1532,13 @@
     </row>
     <row r="11" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" t="s">
         <v>115</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" t="s">
-        <v>117</v>
       </c>
       <c r="D11" t="s">
         <v>74</v>
@@ -1393,21 +1553,21 @@
         <v>77</v>
       </c>
       <c r="H11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s">
         <v>120</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" t="s">
-        <v>122</v>
       </c>
       <c r="D12" t="s">
         <v>76</v>
@@ -1418,13 +1578,13 @@
     </row>
     <row r="13" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
         <v>123</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C13" t="s">
-        <v>125</v>
       </c>
       <c r="D13" t="s">
         <v>76</v>
@@ -1436,29 +1596,27 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="jamessmith@mailinator.com"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="G3" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4"/>
-    <hyperlink ref="G4" r:id="rId5"/>
-    <hyperlink ref="E5" r:id="rId6"/>
-    <hyperlink ref="G5" r:id="rId7"/>
-    <hyperlink ref="E6" r:id="rId8"/>
-    <hyperlink ref="G6" r:id="rId9"/>
-    <hyperlink ref="I7" r:id="rId10"/>
-    <hyperlink ref="G7" r:id="rId11"/>
-    <hyperlink ref="I8" r:id="rId12"/>
-    <hyperlink ref="G8" r:id="rId13"/>
-    <hyperlink ref="E9" r:id="rId14"/>
-    <hyperlink ref="I10" r:id="rId15"/>
-    <hyperlink ref="G10" r:id="rId16"/>
-    <hyperlink ref="K10" r:id="rId17"/>
-    <hyperlink ref="G11" r:id="rId18"/>
-    <hyperlink ref="E11" r:id="rId19"/>
-    <hyperlink ref="E12" r:id="rId20"/>
-    <hyperlink ref="E13" r:id="rId21"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="G5" r:id="rId5"/>
+    <hyperlink ref="E6" r:id="rId6"/>
+    <hyperlink ref="G6" r:id="rId7"/>
+    <hyperlink ref="I7" r:id="rId8"/>
+    <hyperlink ref="G7" r:id="rId9"/>
+    <hyperlink ref="I8" r:id="rId10"/>
+    <hyperlink ref="G8" r:id="rId11"/>
+    <hyperlink ref="E9" r:id="rId12"/>
+    <hyperlink ref="I10" r:id="rId13"/>
+    <hyperlink ref="G10" r:id="rId14"/>
+    <hyperlink ref="K10" r:id="rId15"/>
+    <hyperlink ref="G11" r:id="rId16"/>
+    <hyperlink ref="E11" r:id="rId17"/>
+    <hyperlink ref="E12" r:id="rId18"/>
+    <hyperlink ref="E13" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added different class test cases
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -428,15 +428,6 @@
     <t>phoneNumber</t>
   </si>
   <si>
-    <t>Rohit</t>
-  </si>
-  <si>
-    <t>Yadav</t>
-  </si>
-  <si>
-    <t>rohityadav</t>
-  </si>
-  <si>
     <t>userEmail</t>
   </si>
   <si>
@@ -558,6 +549,15 @@
   </si>
   <si>
     <t>spouseGlaucome</t>
+  </si>
+  <si>
+    <t>Sujeet</t>
+  </si>
+  <si>
+    <t>Verma</t>
+  </si>
+  <si>
+    <t>sujitvarma93</t>
   </si>
 </sst>
 </file>
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1194,19 +1194,19 @@
         <v>124</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
       <c r="F2" t="s">
         <v>125</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="H2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I2" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="J2" t="s">
         <v>129</v>
@@ -1215,34 +1215,34 @@
         <v>126</v>
       </c>
       <c r="L2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M2" s="4">
         <v>1</v>
       </c>
       <c r="N2" t="s">
+        <v>132</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="P2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>134</v>
+      </c>
+      <c r="R2" t="s">
         <v>135</v>
       </c>
-      <c r="O2" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="S2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="T2" t="s">
         <v>136</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="U2" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="R2" t="s">
-        <v>138</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="T2" t="s">
-        <v>139</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.35">
@@ -1253,97 +1253,97 @@
         <v>79</v>
       </c>
       <c r="C3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J3" t="s">
+        <v>145</v>
+      </c>
+      <c r="K3" t="s">
+        <v>146</v>
+      </c>
+      <c r="L3" t="s">
+        <v>147</v>
+      </c>
+      <c r="M3" t="s">
+        <v>148</v>
+      </c>
+      <c r="N3" t="s">
+        <v>168</v>
+      </c>
+      <c r="O3" t="s">
+        <v>149</v>
+      </c>
+      <c r="P3" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R3" t="s">
+        <v>152</v>
+      </c>
+      <c r="S3" t="s">
         <v>169</v>
       </c>
-      <c r="D3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="T3" t="s">
+        <v>153</v>
+      </c>
+      <c r="U3" t="s">
+        <v>154</v>
+      </c>
+      <c r="V3" t="s">
+        <v>155</v>
+      </c>
+      <c r="W3" t="s">
+        <v>156</v>
+      </c>
+      <c r="X3" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AF3" t="s">
         <v>170</v>
       </c>
-      <c r="H3" t="s">
-        <v>146</v>
-      </c>
-      <c r="I3" t="s">
-        <v>147</v>
-      </c>
-      <c r="J3" t="s">
-        <v>148</v>
-      </c>
-      <c r="K3" t="s">
-        <v>149</v>
-      </c>
-      <c r="L3" t="s">
-        <v>150</v>
-      </c>
-      <c r="M3" t="s">
-        <v>151</v>
-      </c>
-      <c r="N3" t="s">
-        <v>171</v>
-      </c>
-      <c r="O3" t="s">
-        <v>152</v>
-      </c>
-      <c r="P3" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>154</v>
-      </c>
-      <c r="R3" t="s">
-        <v>155</v>
-      </c>
-      <c r="S3" t="s">
-        <v>172</v>
-      </c>
-      <c r="T3" t="s">
-        <v>156</v>
-      </c>
-      <c r="U3" t="s">
-        <v>157</v>
-      </c>
-      <c r="V3" t="s">
-        <v>158</v>
-      </c>
-      <c r="W3" t="s">
-        <v>159</v>
-      </c>
-      <c r="X3" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>161</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>163</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>164</v>
-      </c>
-      <c r="AC3" t="s">
+      <c r="AG3" t="s">
         <v>165</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>173</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:73" ht="23" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
added the Medication & Supplements test cases with married user
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -551,13 +551,13 @@
     <t>spouseGlaucome</t>
   </si>
   <si>
-    <t>Sujeet</t>
-  </si>
-  <si>
-    <t>Verma</t>
-  </si>
-  <si>
-    <t>sujitvarma93</t>
+    <t>Nitesh</t>
+  </si>
+  <si>
+    <t>Thakur</t>
+  </si>
+  <si>
+    <t>niteshthakur349</t>
   </si>
 </sst>
 </file>
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added the retirement test cases
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added Real Estate Test cases
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>S.N.</t>
   </si>
@@ -260,154 +260,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>userName/Email</t>
-  </si>
-  <si>
-    <t>jamessmith@mailinator.com</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Password@123</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
     <t>verify_TC003_InvalidLoginWithInvalidPassword</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>verify_TC004_InvalidLoginWithInvalidUserName</t>
-  </si>
-  <si>
-    <t>TC-004</t>
-  </si>
-  <si>
-    <t>jamessmitham@mailinator.com</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>verify_TC005_InvalidLoginWithInvalidUserName_Password</t>
-  </si>
-  <si>
-    <t>TC-005</t>
-  </si>
-  <si>
-    <t>jamessmitham384738@mailinator.com</t>
-  </si>
-  <si>
-    <t>Password@1239876</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>verify_TC006_InvalidLoginWithInvalidUserName_Password_Captcha</t>
-  </si>
-  <si>
-    <t>TC-006</t>
-  </si>
-  <si>
-    <t>jam@essm2ith3am@mailinator.com</t>
-  </si>
-  <si>
-    <t>Pas#$sword@12</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>verify_TC007_ForgotPassword</t>
-  </si>
-  <si>
-    <t>TC-007</t>
-  </si>
-  <si>
-    <t>jasonjohn@mailinator.com</t>
-  </si>
-  <si>
-    <t>newPassword</t>
-  </si>
-  <si>
-    <t>confirmPassword</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>verify_TC008_LoginWithNewPassword</t>
-  </si>
-  <si>
-    <t>TC-008</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>verify_TC009_UnableToForgotPasswordWithInvalidEmail</t>
-  </si>
-  <si>
-    <t>TC-009</t>
-  </si>
-  <si>
-    <t>samhalt@mailinator.com</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>verify_TC010_UnableToLoginOldPassword</t>
-  </si>
-  <si>
-    <t>TC-010</t>
-  </si>
-  <si>
-    <t>danielwatt@mailinator.com</t>
-  </si>
-  <si>
-    <t>Password@12345</t>
-  </si>
-  <si>
-    <t>oldPassword</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>verify_TC011_InvlidLoginWithInvalidCaptcha</t>
-  </si>
-  <si>
-    <t>TC-011</t>
-  </si>
-  <si>
-    <t>captcha</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>verify_TC013_EnterPasswordMasked</t>
-  </si>
-  <si>
-    <t>TC-013</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>verify_TC014_ClickEyeBTPasswordVisible</t>
-  </si>
-  <si>
-    <t>TC-014</t>
   </si>
   <si>
     <t>firstName</t>
@@ -948,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1185,438 +1041,240 @@
         <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2" t="s">
-        <v>173</v>
-      </c>
       <c r="J2" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>126</v>
+        <v>78</v>
       </c>
       <c r="L2" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
       <c r="M2" s="4">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>139</v>
+        <v>91</v>
       </c>
       <c r="P2" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
       <c r="Q2" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="R2" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
       <c r="T2" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="H3" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
       <c r="I3" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="J3" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
       <c r="K3" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="L3" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
       <c r="M3" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="N3" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
       <c r="O3" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="P3" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="Q3" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="R3" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
       <c r="S3" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="T3" t="s">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="U3" t="s">
-        <v>154</v>
+        <v>106</v>
       </c>
       <c r="V3" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="W3" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="X3" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="Y3" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="Z3" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="AA3" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="AB3" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
       <c r="AC3" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
       <c r="AD3" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
       <c r="AE3" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
       <c r="AF3" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="AG3" t="s">
-        <v>165</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:73" ht="23" x14ac:dyDescent="0.5">
-      <c r="A4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="6"/>
       <c r="M4" s="1"/>
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="6"/>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>93</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="6"/>
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" t="s">
-        <v>99</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="5"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="I7" s="3"/>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" t="s">
-        <v>99</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="5"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>106</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="5"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H10" t="s">
-        <v>99</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="J10" t="s">
-        <v>112</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="5"/>
+      <c r="E10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C11" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H11" t="s">
-        <v>116</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="5"/>
+      <c r="E11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="5"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:73" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="5"/>
+      <c r="E13" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="jamessmith@mailinator.com"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="G5" r:id="rId5"/>
-    <hyperlink ref="E6" r:id="rId6"/>
-    <hyperlink ref="G6" r:id="rId7"/>
-    <hyperlink ref="I7" r:id="rId8"/>
-    <hyperlink ref="G7" r:id="rId9"/>
-    <hyperlink ref="I8" r:id="rId10"/>
-    <hyperlink ref="G8" r:id="rId11"/>
-    <hyperlink ref="E9" r:id="rId12"/>
-    <hyperlink ref="I10" r:id="rId13"/>
-    <hyperlink ref="G10" r:id="rId14"/>
-    <hyperlink ref="K10" r:id="rId15"/>
-    <hyperlink ref="G11" r:id="rId16"/>
-    <hyperlink ref="E11" r:id="rId17"/>
-    <hyperlink ref="E12" r:id="rId18"/>
-    <hyperlink ref="E13" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added the finance test cases
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -296,9 +296,6 @@
     <t>spouseFirstName</t>
   </si>
   <si>
-    <t>Radha</t>
-  </si>
-  <si>
     <t>spouseDob</t>
   </si>
   <si>
@@ -407,13 +404,16 @@
     <t>spouseGlaucome</t>
   </si>
   <si>
-    <t>Nitesh</t>
-  </si>
-  <si>
-    <t>Thakur</t>
-  </si>
-  <si>
-    <t>niteshthakur349</t>
+    <t>Rishi</t>
+  </si>
+  <si>
+    <t>Nigam</t>
+  </si>
+  <si>
+    <t>rishinigam23</t>
+  </si>
+  <si>
+    <t>Richa</t>
   </si>
 </sst>
 </file>
@@ -804,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1050,19 +1050,19 @@
         <v>76</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
         <v>77</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H2" t="s">
         <v>82</v>
       </c>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J2" t="s">
         <v>81</v>
@@ -1080,25 +1080,25 @@
         <v>84</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P2" t="s">
         <v>85</v>
       </c>
       <c r="Q2" t="s">
+        <v>125</v>
+      </c>
+      <c r="R2" t="s">
         <v>86</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T2" t="s">
         <v>87</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="U2" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.35">
@@ -1109,97 +1109,97 @@
         <v>75</v>
       </c>
       <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
         <v>118</v>
       </c>
-      <c r="D3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>94</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" t="s">
+        <v>99</v>
+      </c>
+      <c r="N3" t="s">
         <v>119</v>
       </c>
-      <c r="H3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I3" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3" t="s">
-        <v>98</v>
-      </c>
-      <c r="L3" t="s">
-        <v>99</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>100</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>102</v>
+      </c>
+      <c r="R3" t="s">
+        <v>103</v>
+      </c>
+      <c r="S3" t="s">
         <v>120</v>
       </c>
-      <c r="O3" t="s">
-        <v>101</v>
-      </c>
-      <c r="P3" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>103</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>104</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
+        <v>105</v>
+      </c>
+      <c r="V3" t="s">
+        <v>106</v>
+      </c>
+      <c r="W3" t="s">
+        <v>107</v>
+      </c>
+      <c r="X3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF3" t="s">
         <v>121</v>
       </c>
-      <c r="T3" t="s">
-        <v>105</v>
-      </c>
-      <c r="U3" t="s">
-        <v>106</v>
-      </c>
-      <c r="V3" t="s">
-        <v>107</v>
-      </c>
-      <c r="W3" t="s">
-        <v>108</v>
-      </c>
-      <c r="X3" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>116</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>122</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:73" ht="23" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
Revert "Merge pull request #27 from AgingOptions-com/HealthInfo"
This reverts commit f8eb37ba407566d8c33c50beb39f4e2c8988b3ea, reversing
changes made to e18a48484276a694da84fe5c2375477ca02dd827.
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -296,6 +296,9 @@
     <t>spouseFirstName</t>
   </si>
   <si>
+    <t>Radha</t>
+  </si>
+  <si>
     <t>spouseDob</t>
   </si>
   <si>
@@ -404,16 +407,13 @@
     <t>spouseGlaucome</t>
   </si>
   <si>
-    <t>Rishi</t>
-  </si>
-  <si>
-    <t>Nigam</t>
-  </si>
-  <si>
-    <t>rishinigam23</t>
-  </si>
-  <si>
-    <t>Richa</t>
+    <t>Nitesh</t>
+  </si>
+  <si>
+    <t>Thakur</t>
+  </si>
+  <si>
+    <t>niteshthakur349</t>
   </si>
 </sst>
 </file>
@@ -804,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1050,19 +1050,19 @@
         <v>76</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
         <v>77</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H2" t="s">
         <v>82</v>
       </c>
       <c r="I2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J2" t="s">
         <v>81</v>
@@ -1080,25 +1080,25 @@
         <v>84</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P2" t="s">
         <v>85</v>
       </c>
       <c r="Q2" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="R2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="S2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T2" t="s">
+        <v>88</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="T2" t="s">
-        <v>87</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.35">
@@ -1109,97 +1109,97 @@
         <v>75</v>
       </c>
       <c r="C3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" t="s">
+        <v>99</v>
+      </c>
+      <c r="M3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" t="s">
+        <v>120</v>
+      </c>
+      <c r="O3" t="s">
+        <v>101</v>
+      </c>
+      <c r="P3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" t="s">
+        <v>104</v>
+      </c>
+      <c r="S3" t="s">
+        <v>121</v>
+      </c>
+      <c r="T3" t="s">
+        <v>105</v>
+      </c>
+      <c r="U3" t="s">
+        <v>106</v>
+      </c>
+      <c r="V3" t="s">
+        <v>107</v>
+      </c>
+      <c r="W3" t="s">
+        <v>108</v>
+      </c>
+      <c r="X3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG3" t="s">
         <v>117</v>
-      </c>
-      <c r="D3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" t="s">
-        <v>118</v>
-      </c>
-      <c r="H3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" t="s">
-        <v>96</v>
-      </c>
-      <c r="K3" t="s">
-        <v>97</v>
-      </c>
-      <c r="L3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" t="s">
-        <v>99</v>
-      </c>
-      <c r="N3" t="s">
-        <v>119</v>
-      </c>
-      <c r="O3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P3" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>102</v>
-      </c>
-      <c r="R3" t="s">
-        <v>103</v>
-      </c>
-      <c r="S3" t="s">
-        <v>120</v>
-      </c>
-      <c r="T3" t="s">
-        <v>104</v>
-      </c>
-      <c r="U3" t="s">
-        <v>105</v>
-      </c>
-      <c r="V3" t="s">
-        <v>106</v>
-      </c>
-      <c r="W3" t="s">
-        <v>107</v>
-      </c>
-      <c r="X3" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>109</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>115</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:73" ht="23" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
added finance test cases
</commit_message>
<xml_diff>
--- a/agingoptions/src/main/resources/TestData.xlsx
+++ b/agingoptions/src/main/resources/TestData.xlsx
@@ -407,13 +407,13 @@
     <t>spouseGlaucome</t>
   </si>
   <si>
-    <t>Nitesh</t>
-  </si>
-  <si>
-    <t>Thakur</t>
-  </si>
-  <si>
-    <t>niteshthakur349</t>
+    <t>Hitesh</t>
+  </si>
+  <si>
+    <t>Verma</t>
+  </si>
+  <si>
+    <t>hiteshverma349</t>
   </si>
 </sst>
 </file>
@@ -804,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>